<commit_message>
logIn now works ends if login window closed and not logged in
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -1,88 +1,98 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
-  <workbookPr/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588D365B-19BC-4093-BA04-5D0BDF1FFDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Staff" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF743E2-3C25-47BB-8717-06E08B619FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <x:bookViews>
+    <x:workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Staff" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="162913"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Nathan</t>
-  </si>
-  <si>
-    <t>Alana</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:si>
+    <x:t>NATHAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALANA</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </x:cellStyleXfs>
+  <x:cellXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -347,32 +357,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>4321</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B2"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A3" sqref="A3"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0">
+        <x:v>1234</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B2" s="0">
+        <x:v>4321</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
moves staff to edit to create staff
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -1,15 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <x:workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2C6369-BEB8-499C-84D1-20A02D509061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Staff" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Staff" sheetId="2" r:id="rId1"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="0"/>
 </x:workbook>
 </file>
 
@@ -21,17 +28,25 @@
   <x:si>
     <x:t>1111</x:t>
   </x:si>
+  <x:si>
+    <x:t>NATHAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DANSKIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MANAGER</x:t>
+  </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="1" x14ac:knownFonts="1">
     <x:font>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -47,38 +62,36 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -366,17 +379,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D1"/>
+  <x:dimension ref="A1:D2"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="C2" sqref="C2"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="8.424911" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="8.996339" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="4.996339" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="10.139196" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
+    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -388,12 +409,26 @@
       </x:c>
       <x:c r="D1" s="0" t="s">
         <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C2" s="1">
+        <x:v>2222</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>4</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>

</xml_diff>

<commit_message>
delete staff from excel remove staff from editing cannot remove admin cannot remove if logged in
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2C6369-BEB8-499C-84D1-20A02D509061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0921C66F-7AAF-4EAC-B2D2-243A10ADA429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -33,6 +33,9 @@
   </x:si>
   <x:si>
     <x:t>DANSKIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2222</x:t>
   </x:si>
   <x:si>
     <x:t>MANAGER</x:t>
@@ -386,7 +389,7 @@
   <x:dimension ref="A1:D2"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="C2" sqref="C2"/>
+      <x:selection activeCell="A3" sqref="A3"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,17 +421,17 @@
       <x:c r="B2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C2" s="1">
-        <x:v>2222</x:v>
+      <x:c r="C2" s="1" t="s">
+        <x:v>4</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>

</xml_diff>

<commit_message>
clears staff box select and removes row from excel
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0921C66F-7AAF-4EAC-B2D2-243A10ADA429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408A4375-7003-48AC-B195-80F555C2BEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -29,16 +29,13 @@
     <x:t>1111</x:t>
   </x:si>
   <x:si>
-    <x:t>NATHAN</x:t>
+    <x:t>ALANA</x:t>
   </x:si>
   <x:si>
     <x:t>DANSKIN</x:t>
   </x:si>
   <x:si>
-    <x:t>2222</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MANAGER</x:t>
+    <x:t>STAFF</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -73,15 +70,11 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
+  <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,18 +379,18 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D2"/>
+  <x:dimension ref="A1:D3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A3" sqref="A3"/>
+      <x:selection activeCell="A4" sqref="A4 A3"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="8.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="7.424911" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="8.996339" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="10.139196" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="7.424911" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -421,11 +414,11 @@
       <x:c r="B2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C2" s="1" t="s">
+      <x:c r="C2" s="0">
+        <x:v>3333</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
         <x:v>4</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
save new staff to new row doesnt check the bool yet for exist
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408A4375-7003-48AC-B195-80F555C2BEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2305F474-C919-46A7-BA59-387A6DFF4B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -36,6 +36,18 @@
   </x:si>
   <x:si>
     <x:t>STAFF</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NATHAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DANKSIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MANAGER</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2222</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -382,15 +394,15 @@
   <x:dimension ref="A1:D3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A4" sqref="A4 A3"/>
+      <x:selection activeCell="D4" sqref="D4"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="7.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="8.424911" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="8.996339" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="7.424911" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="10.139196" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -419,6 +431,34 @@
       </x:c>
       <x:c r="D2" s="0" t="s">
         <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C3" s="0">
+        <x:v>2222</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="A4" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
adds staff to excel and checks to see if it matches pin or names
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -1,106 +1,94 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <x:workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2305F474-C919-46A7-BA59-387A6DFF4B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Staff" sheetId="2" r:id="rId1"/>
-  </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="0"/>
-</x:workbook>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F0D40F-7D5C-4B25-8664-7486B5924B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Staff" sheetId="2" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="0"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:si>
-    <x:t>ADMIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1111</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ALANA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DANSKIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STAFF</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NATHAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DANKSIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MANAGER</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2222</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>NATHAN</t>
+  </si>
+  <si>
+    <t>DANSKIN</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="1" x14ac:knownFonts="1">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-  </x:cellStyleXfs>
-  <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
-</x:styleSheet>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,85 +375,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:D3"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="D4" sqref="D4"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:cols>
-    <x:col min="1" max="1" width="8.424911" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="8.996339" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="10.139196" style="0" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C2" s="0">
-        <x:v>3333</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C3" s="0">
-        <x:v>2222</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="A4" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>2222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
still closes after staff add didnt remove staff after delete
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -1,94 +1,97 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F0D40F-7D5C-4B25-8664-7486B5924B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Staff" sheetId="2" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="0"/>
-</workbook>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E28A83-5B0D-46C6-8890-EBEA1DF18A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <x:bookViews>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Staff" sheetId="2" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="0"/>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
-  <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>1111</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>NATHAN</t>
-  </si>
-  <si>
-    <t>DANSKIN</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:si>
+    <x:t>ADMIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1111</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NATHAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DANSKIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>D</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="1" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  </x:cellStyleXfs>
+  <x:cellXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,57 +378,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>2222</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E2"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A3" sqref="A3"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="8.424911" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="8.996339" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="4.996339" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="7.424911" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="2.282054" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" s="0">
+        <x:v>2222</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
check names and id works now adjust colors
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -1,97 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <x:workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E28A83-5B0D-46C6-8890-EBEA1DF18A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Staff" sheetId="2" r:id="rId1"/>
-  </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="0"/>
-</x:workbook>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CCE833-AF4F-4C12-A873-E7FE859A01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Staff" sheetId="2" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="0"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:si>
-    <x:t>ADMIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1111</x:t>
-  </x:si>
-  <x:si>
-    <x:t>A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NATHAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DANSKIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>D</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>NATHAN</t>
+  </si>
+  <si>
+    <t>DANSKIN</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="1" x14ac:knownFonts="1">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-  </x:cellStyleXfs>
-  <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
-</x:styleSheet>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,64 +369,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:E2"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A3" sqref="A3"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:cols>
-    <x:col min="1" max="1" width="8.424911" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="8.996339" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="7.424911" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="2.282054" style="0" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E1" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C2" s="0">
-        <x:v>2222</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change color with mathcing but closes without changing back to match if last match
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CCE833-AF4F-4C12-A873-E7FE859A01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A794DF-A2CB-4ADF-BA0E-7C93871D457E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -373,7 +373,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updates time and date on login and ill screen with current values
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -39,18 +39,6 @@
   </x:si>
   <x:si>
     <x:t>MANAGER</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ALANA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TEAR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6666</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STAFF</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -397,7 +385,7 @@
   <x:dimension ref="A1:D2"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="F6" sqref="F6 F4 F5"/>
+      <x:selection activeCell="F6" sqref="F6 F2 F3 F4 F5"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +410,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -434,20 +422,6 @@
       </x:c>
       <x:c r="D2" s="0" t="s">
         <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="A3" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>9</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
added sorting to excel file for when creating the staff list will automatically be in alphabetical order. will need to add to staff edit: var range = workSheet.Range(strXlsxStaffNameColumn + 1, strXlsxStaffRoleColumn + workSheet.RowsUsed().Count()); range.SetAutoFilter().Sort(2, XLSortOrder.Ascending); in order to resave but call autofilter.reapply()
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -1,55 +1,65 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4527E227-16F4-4D1B-B31F-E9B622288285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Staff" sheetId="2" r:id="rId1"/>
+    <x:sheet name="Staff" sheetId="2" r:id="rId2"/>
   </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="0"/>
+  <x:definedNames>
+    <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Staff!$A$1:$D$4</x:definedName>
+  </x:definedNames>
+  <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
+    <x:t>FIRST NAME</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LAST NAME</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CODE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ROLE</x:t>
+  </x:si>
+  <x:si>
     <x:t>ADMIN</x:t>
   </x:si>
   <x:si>
     <x:t>1111</x:t>
   </x:si>
   <x:si>
-    <x:t>NATHAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DANSKIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MANAGER</x:t>
+    <x:t>dead</x:t>
+  </x:si>
+  <x:si>
+    <x:t>roll</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1" x14ac:knownFonts="1">
+  <x:fonts count="2">
     <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -65,32 +75,45 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -378,53 +401,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D2"/>
+  <x:dimension ref="A1:D4"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="F6" sqref="F6 F2 F3 F4 F5"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="8.424911" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="8.996339" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="10.139196" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="11.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="10.996339" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="5.853482" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="7.424911" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="0" t="s">
+    <x:row r="1" spans="1:4" s="1" customFormat="1">
+      <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
+      <x:c r="B1" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>0</x:v>
+      <x:c r="C1" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="1" t="s">
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>5</x:v>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="B3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="B4" s="0" t="s">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
+  <x:autoFilter ref="A1:D4">
+    <x:sortState ref="A2:D4">
+      <x:sortCondition ref="B1:B4"/>
+    </x:sortState>
+  </x:autoFilter>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>

<commit_message>
combo box changed to stack panel sets and saves from excel makes new stack buttons
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -1,123 +1,114 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:workbookPr codeName="ThisWorkbook"/>
-  <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Staff" sheetId="2" r:id="rId2"/>
-  </x:sheets>
-  <x:definedNames>
-    <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Staff!$A$1:$D$3</x:definedName>
-  </x:definedNames>
-  <x:calcPr calcId="125725"/>
-</x:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814A7A1C-6398-4CB2-AB60-410C7AE81B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Staff" sheetId="2" r:id="rId1"/>
+  </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Staff!$A$1:$D$3</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:si>
-    <x:t>FIRST NAME</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LAST NAME</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CODE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ROLE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ADMIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1111</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NATHAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DANSKIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2222</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+  <si>
+    <t>FIRST NAME</t>
+  </si>
+  <si>
+    <t>LAST NAME</t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>ROLE</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>NATHAN</t>
+  </si>
+  <si>
+    <t>DANSKIN</t>
+  </si>
+  <si>
+    <t>2222</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="2">
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-    <x:font>
-      <x:b/>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellStyleXfs>
-  <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-</x:styleSheet>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -404,74 +395,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:D2"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:cols>
-    <x:col min="1" max="1" width="13.996339" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="13.282054" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="8.139196" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="7.710625" style="0" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:4" s="1" customFormat="1">
-      <x:c r="A1" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="1" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="A3" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:autoFilter ref="A1:D3">
-    <x:sortState ref="A2:D3">
-      <x:sortCondition ref="B1:B3"/>
-    </x:sortState>
-  </x:autoFilter>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D3" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D3">
+      <sortCondition ref="B1:B3"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tgl buttons now do data edit deletes button and excel row add to edit field to alter and save
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -1,114 +1,128 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814A7A1C-6398-4CB2-AB60-410C7AE81B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Staff" sheetId="2" r:id="rId1"/>
-  </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Staff!$A$1:$D$3</definedName>
-  </definedNames>
-  <calcPr calcId="0"/>
-</workbook>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FB6D81-46DF-48AE-8DBF-19D354A88C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <x:bookViews>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Staff" sheetId="2" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames>
+    <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Staff!$A$1:$D$4</x:definedName>
+  </x:definedNames>
+  <x:calcPr calcId="0"/>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
-  <si>
-    <t>FIRST NAME</t>
-  </si>
-  <si>
-    <t>LAST NAME</t>
-  </si>
-  <si>
-    <t>CODE</t>
-  </si>
-  <si>
-    <t>ROLE</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>1111</t>
-  </si>
-  <si>
-    <t>NATHAN</t>
-  </si>
-  <si>
-    <t>DANSKIN</t>
-  </si>
-  <si>
-    <t>2222</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:si>
+    <x:t>FIRST NAME</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LAST NAME</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CODE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ROLE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ADMIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1111</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NATHAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DANSKIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2222</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALANA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3333</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MANAGER</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-  </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -395,69 +409,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:D3" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D3">
-      <sortCondition ref="B1:B3"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:D3"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="B4" sqref="B4 B3"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="13.996339" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="13.282054" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="8.139196" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="10.139196" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="A4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:autoFilter ref="A1:D4">
+    <x:sortState ref="A2:D4">
+      <x:sortCondition ref="B1:B4"/>
+    </x:sortState>
+  </x:autoFilter>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
checks staff enter for blank space changes colour of text box to red if emptty
</commit_message>
<xml_diff>
--- a/Resources/StaffID.xlsx
+++ b/Resources/StaffID.xlsx
@@ -1,131 +1,126 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <x:workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FB6D81-46DF-48AE-8DBF-19D354A88C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Staff" sheetId="2" r:id="rId1"/>
-  </x:sheets>
-  <x:definedNames>
-    <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Staff!$A$1:$D$4</x:definedName>
-  </x:definedNames>
-  <x:calcPr calcId="0"/>
-</x:workbook>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DA8D8E-5B1E-4244-BE1F-5C3DCB185367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Staff" sheetId="2" r:id="rId1"/>
+  </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Staff!$A$1:$D$4</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:si>
-    <x:t>FIRST NAME</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LAST NAME</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CODE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ROLE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ADMIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1111</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ALANA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DANSKIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3333</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MANAGER</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NATHAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TEST</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2222</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+  <si>
+    <t>FIRST NAME</t>
+  </si>
+  <si>
+    <t>LAST NAME</t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>ROLE</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>ALANA</t>
+  </si>
+  <si>
+    <t>DANSKIN</t>
+  </si>
+  <si>
+    <t>3333</t>
+  </si>
+  <si>
+    <t>MANAGER</t>
+  </si>
+  <si>
+    <t>NATHAN</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>2222</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="2" x14ac:knownFonts="1">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-    <x:font>
-      <x:b/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellStyleXfs>
-  <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
-</x:styleSheet>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,90 +407,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:D3"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="B4" sqref="B4 B3"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:cols>
-    <x:col min="1" max="1" width="13.996339" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="13.282054" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="8.139196" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="10.139196" style="0" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="1" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="A3" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="A4" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:autoFilter ref="A1:D4">
-    <x:sortState ref="A2:D4">
-      <x:sortCondition ref="B1:B4"/>
-    </x:sortState>
-  </x:autoFilter>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D4" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D4">
+      <sortCondition ref="B1:B4"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
 </file>
</xml_diff>